<commit_message>
Update with recent changes before initial release of thermostat project on hackster.io
</commit_message>
<xml_diff>
--- a/documents/SmartVentPrototypeArea.xlsx
+++ b/documents/SmartVentPrototypeArea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedtoal/Documents/Writings/Technical Docs/928 Lighthouse Drive/SmartVent Thermostat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7E2D3B-CB9F-DF47-98FD-47DCC0978A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6EDB7C-7817-F144-9694-302BA1EA2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6160" yWindow="2240" windowWidth="41440" windowHeight="24280" xr2:uid="{1775EFD8-74DA-2F4D-8AD4-A113DBB4D7AA}"/>
   </bookViews>
@@ -425,9 +425,6 @@
     <t>Indoor Thermistor</t>
   </si>
   <si>
-    <t>K3,L4,L6,Nano5</t>
-  </si>
-  <si>
     <t>Relay Activate</t>
   </si>
   <si>
@@ -458,7 +455,10 @@
     <t>Outdoor Sensor 1</t>
   </si>
   <si>
-    <t>K9,K4,L5,M4,N4,Nano3,Nano24</t>
+    <t>K3,L5,L6,Nano5</t>
+  </si>
+  <si>
+    <t>K9,K4,L4,M4,N4,Nano3,Nano24</t>
   </si>
 </sst>
 </file>
@@ -1028,28 +1028,58 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1076,34 +1106,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1119,18 +1131,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1550,11 +1550,11 @@
       <c r="N3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="86" t="s">
+      <c r="O3" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="76"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="72"/>
       <c r="R3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1564,25 +1564,25 @@
       <c r="T3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="U3" s="75" t="s">
+      <c r="U3" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="V3" s="75"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="81" t="s">
+      <c r="V3" s="71"/>
+      <c r="W3" s="72"/>
+      <c r="X3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="Y3" s="80" t="s">
+      <c r="Y3" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" s="80"/>
+      <c r="Z3" s="90"/>
       <c r="AA3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AB3" s="75" t="s">
+      <c r="AB3" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="AC3" s="75"/>
+      <c r="AC3" s="71"/>
       <c r="AD3" s="31" t="s">
         <v>0</v>
       </c>
@@ -1615,11 +1615,11 @@
       <c r="Q4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="R4" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
       <c r="U4" s="25" t="s">
         <v>0</v>
       </c>
@@ -1627,19 +1627,19 @@
       <c r="W4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="X4" s="82"/>
+      <c r="X4" s="92"/>
       <c r="Y4" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="Z4" s="75" t="s">
+      <c r="Z4" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="AA4" s="75"/>
-      <c r="AB4" s="75"/>
+      <c r="AA4" s="71"/>
+      <c r="AB4" s="71"/>
       <c r="AC4" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="AD4" s="78" t="str">
+      <c r="AD4" s="88" t="str">
         <f>"+
 D4
 -"</f>
@@ -1669,40 +1669,40 @@
       <c r="N5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="87" t="s">
+      <c r="O5" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="77"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="75"/>
       <c r="R5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="S5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="T5" s="89" t="s">
+      <c r="T5" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="U5" s="71" t="s">
+      <c r="U5" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="V5" s="71"/>
-      <c r="W5" s="77"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="75"/>
       <c r="X5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="Y5" s="75" t="s">
+      <c r="Y5" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="Z5" s="76"/>
+      <c r="Z5" s="72"/>
       <c r="AA5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="AB5" s="75" t="s">
+      <c r="AB5" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="AC5" s="76"/>
-      <c r="AD5" s="79"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="89"/>
       <c r="AE5" s="24">
         <v>3</v>
       </c>
@@ -1726,30 +1726,30 @@
         <f>"+"</f>
         <v>+</v>
       </c>
-      <c r="O6" s="72" t="s">
+      <c r="O6" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="72"/>
+      <c r="P6" s="77"/>
       <c r="Q6" s="17" t="str">
         <f>"-"</f>
         <v>-</v>
       </c>
-      <c r="R6" s="90" t="s">
+      <c r="R6" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="92" t="s">
+      <c r="S6" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="T6" s="89"/>
+      <c r="T6" s="81"/>
       <c r="U6" s="3" t="str">
         <f>"+"</f>
         <v>+</v>
       </c>
-      <c r="V6" s="72" t="s">
+      <c r="V6" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="W6" s="72"/>
-      <c r="X6" s="73"/>
+      <c r="W6" s="77"/>
+      <c r="X6" s="80"/>
       <c r="Y6" s="15" t="str">
         <f>"-"</f>
         <v>-</v>
@@ -1795,16 +1795,16 @@
         <f>"+"</f>
         <v>+</v>
       </c>
-      <c r="O7" s="75" t="s">
+      <c r="O7" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="75"/>
+      <c r="P7" s="71"/>
       <c r="Q7" s="15" t="str">
         <f>"-"</f>
         <v>-</v>
       </c>
-      <c r="R7" s="91"/>
-      <c r="S7" s="93"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="85"/>
       <c r="T7" s="46" t="s">
         <v>74</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="AC7" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="AD7" s="70" t="s">
+      <c r="AD7" s="78" t="s">
         <v>32</v>
       </c>
       <c r="AE7" s="24">
@@ -1859,31 +1859,31 @@
       <c r="O8" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
       <c r="S8" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="74" t="s">
+      <c r="T8" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="U8" s="72"/>
-      <c r="V8" s="72"/>
-      <c r="W8" s="70"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="78"/>
       <c r="X8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Y8" s="74" t="s">
+      <c r="Y8" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="Z8" s="72"/>
-      <c r="AA8" s="72"/>
-      <c r="AB8" s="72"/>
-      <c r="AC8" s="70"/>
-      <c r="AD8" s="70"/>
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="77"/>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="78"/>
+      <c r="AD8" s="78"/>
       <c r="AE8" s="24">
         <v>6</v>
       </c>
@@ -1903,24 +1903,24 @@
       <c r="M9" s="56">
         <v>7</v>
       </c>
-      <c r="N9" s="94" t="s">
+      <c r="N9" s="86" t="s">
         <v>53</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="73" t="s">
+      <c r="P9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
       <c r="S9" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="T9" s="74"/>
-      <c r="U9" s="72"/>
-      <c r="V9" s="72"/>
-      <c r="W9" s="70"/>
+      <c r="T9" s="76"/>
+      <c r="U9" s="77"/>
+      <c r="V9" s="77"/>
+      <c r="W9" s="78"/>
       <c r="X9" s="19" t="s">
         <v>0</v>
       </c>
@@ -1957,15 +1957,15 @@
       <c r="M10" s="56">
         <v>8</v>
       </c>
-      <c r="N10" s="95"/>
+      <c r="N10" s="87"/>
       <c r="O10" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="P10" s="75" t="s">
+      <c r="P10" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="75"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
       <c r="S10" s="14" t="s">
         <v>0</v>
       </c>
@@ -1981,11 +1981,11 @@
       <c r="W10" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="X10" s="83" t="s">
+      <c r="X10" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Y10" s="80"/>
-      <c r="Z10" s="80"/>
+      <c r="Y10" s="90"/>
+      <c r="Z10" s="90"/>
       <c r="AA10" s="16" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +1995,7 @@
       <c r="AC10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD10" s="78" t="str">
+      <c r="AD10" s="88" t="str">
         <f>"+
 D5
 -"</f>
@@ -2052,9 +2052,9 @@
       <c r="W11" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="X11" s="84"/>
-      <c r="Y11" s="80"/>
-      <c r="Z11" s="80"/>
+      <c r="X11" s="94"/>
+      <c r="Y11" s="90"/>
+      <c r="Z11" s="90"/>
       <c r="AA11" s="53" t="s">
         <v>76</v>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="AC11" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="AD11" s="79"/>
+      <c r="AD11" s="89"/>
       <c r="AE11" s="24">
         <v>9</v>
       </c>
@@ -2114,16 +2114,16 @@
       <c r="W12" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="X12" s="84"/>
-      <c r="Y12" s="80"/>
-      <c r="Z12" s="85"/>
+      <c r="X12" s="94"/>
+      <c r="Y12" s="90"/>
+      <c r="Z12" s="95"/>
       <c r="AA12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="AB12" s="71" t="s">
+      <c r="AB12" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="AC12" s="71"/>
+      <c r="AC12" s="74"/>
       <c r="AD12" s="31" t="s">
         <v>0</v>
       </c>
@@ -2206,14 +2206,14 @@
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="88" t="s">
+      <c r="J14" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
@@ -2231,12 +2231,12 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
@@ -2254,12 +2254,12 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="79"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="25"/>
@@ -2560,6 +2560,20 @@
     <row r="46" spans="2:33" ht="100" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AD4:AD5"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="X10:Z12"/>
+    <mergeCell ref="AD10:AD11"/>
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="T8:W9"/>
@@ -2575,20 +2589,6 @@
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="AD4:AD5"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="X10:Z12"/>
-    <mergeCell ref="AD10:AD11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="21" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -2695,25 +2695,25 @@
       <c r="C3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="73"/>
+      <c r="E3" s="80"/>
       <c r="F3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="103" t="s">
+      <c r="G3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="104"/>
-      <c r="I3" s="81" t="s">
+      <c r="H3" s="99"/>
+      <c r="I3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="86" t="s">
+      <c r="J3" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="75"/>
-      <c r="L3" s="76"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="72"/>
       <c r="M3" s="14" t="s">
         <v>0</v>
       </c>
@@ -2723,11 +2723,11 @@
       <c r="O3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="86" t="s">
+      <c r="P3" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="76"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="72"/>
       <c r="S3" s="37" t="s">
         <v>0</v>
       </c>
@@ -2743,7 +2743,7 @@
       <c r="B4" s="9">
         <v>2</v>
       </c>
-      <c r="C4" s="78" t="str">
+      <c r="C4" s="88" t="str">
         <f>"+
 D4
 -"</f>
@@ -2754,15 +2754,15 @@
       <c r="D4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="73" t="s">
+      <c r="E4" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="82"/>
+      <c r="I4" s="92"/>
       <c r="J4" s="16" t="s">
         <v>0</v>
       </c>
@@ -2772,11 +2772,11 @@
       <c r="L4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="73" t="s">
+      <c r="M4" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
       <c r="P4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2801,27 +2801,27 @@
       <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="86" t="s">
+      <c r="C5" s="96"/>
+      <c r="D5" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="75"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="75"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="87" t="s">
+      <c r="J5" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="94" t="s">
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="86" t="s">
         <v>69</v>
       </c>
       <c r="N5" s="19" t="s">
@@ -2830,11 +2830,11 @@
       <c r="O5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="87" t="s">
+      <c r="P5" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="77"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="75"/>
       <c r="S5" s="33" t="s">
         <v>0</v>
       </c>
@@ -2868,29 +2868,29 @@
       <c r="H6" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
       <c r="L6" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="M6" s="95"/>
-      <c r="N6" s="98" t="s">
+      <c r="M6" s="87"/>
+      <c r="N6" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="O6" s="97" t="s">
+      <c r="O6" s="101" t="s">
         <v>43</v>
       </c>
       <c r="P6" s="16" t="str">
         <f>"-"</f>
         <v>-</v>
       </c>
-      <c r="Q6" s="72" t="s">
+      <c r="Q6" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="72"/>
+      <c r="R6" s="77"/>
       <c r="S6" s="15" t="str">
         <f>"+"</f>
         <v>+</v>
@@ -2917,7 +2917,7 @@
       <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="C7" s="102" t="s">
+      <c r="C7" s="97" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="46" t="s">
@@ -2946,16 +2946,16 @@
       <c r="M7" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="99"/>
-      <c r="O7" s="71"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="74"/>
       <c r="P7" s="18" t="str">
         <f>"-"</f>
         <v>-</v>
       </c>
-      <c r="Q7" s="71" t="s">
+      <c r="Q7" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="R7" s="71"/>
+      <c r="R7" s="74"/>
       <c r="S7" s="28" t="str">
         <f>"+"</f>
         <v>+</v>
@@ -2982,31 +2982,31 @@
       <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="74" t="s">
+      <c r="C8" s="97"/>
+      <c r="D8" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="70"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="78"/>
       <c r="I8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="74" t="s">
+      <c r="J8" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="70"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="78"/>
       <c r="N8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="71"/>
-      <c r="Q8" s="71"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
       <c r="R8" s="28" t="s">
         <v>0</v>
       </c>
@@ -3042,22 +3042,22 @@
       <c r="I9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="70"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="78"/>
       <c r="N9" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="73" t="s">
+      <c r="O9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
       <c r="R9" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="S9" s="94" t="s">
+      <c r="S9" s="86" t="s">
         <v>53</v>
       </c>
       <c r="T9" s="56">
@@ -3072,7 +3072,7 @@
       <c r="B10" s="9">
         <v>8</v>
       </c>
-      <c r="C10" s="78" t="str">
+      <c r="C10" s="88" t="str">
         <f>"+
 D5
 -"</f>
@@ -3089,11 +3089,11 @@
       <c r="F10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="84" t="s">
+      <c r="G10" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="80"/>
-      <c r="I10" s="100"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="104"/>
       <c r="J10" s="42" t="s">
         <v>71</v>
       </c>
@@ -3109,15 +3109,15 @@
       <c r="N10" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="75" t="s">
+      <c r="O10" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="73"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="80"/>
       <c r="R10" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="S10" s="95"/>
+      <c r="S10" s="87"/>
       <c r="T10" s="56">
         <v>8</v>
       </c>
@@ -3130,7 +3130,7 @@
       <c r="B11" s="9">
         <v>9</v>
       </c>
-      <c r="C11" s="96"/>
+      <c r="C11" s="100"/>
       <c r="D11" s="55" t="s">
         <v>75</v>
       </c>
@@ -3140,9 +3140,9 @@
       <c r="F11" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="84"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="85"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="95"/>
       <c r="J11" s="29" t="s">
         <v>0</v>
       </c>
@@ -3191,16 +3191,16 @@
       <c r="C12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="71"/>
+      <c r="E12" s="74"/>
       <c r="F12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="84"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="85"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="95"/>
       <c r="J12" s="26" t="s">
         <v>44</v>
       </c>
@@ -3321,14 +3321,14 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="88" t="s">
+      <c r="R14" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="S14" s="88"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="88"/>
-      <c r="V14" s="88"/>
-      <c r="W14" s="88"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="79"/>
+      <c r="U14" s="79"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="79"/>
       <c r="AE14" s="6"/>
       <c r="AG14" s="66" t="s">
         <v>89</v>
@@ -3351,12 +3351,12 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="88"/>
-      <c r="U15" s="88"/>
-      <c r="V15" s="88"/>
-      <c r="W15" s="88"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="79"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="79"/>
       <c r="AE15" s="6"/>
       <c r="AH15" s="64" t="s">
         <v>90</v>
@@ -3379,12 +3379,12 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="88"/>
-      <c r="U16" s="88"/>
-      <c r="V16" s="88"/>
-      <c r="W16" s="88"/>
+      <c r="R16" s="79"/>
+      <c r="S16" s="79"/>
+      <c r="T16" s="79"/>
+      <c r="U16" s="79"/>
+      <c r="V16" s="79"/>
+      <c r="W16" s="79"/>
       <c r="AE16" s="6"/>
       <c r="AG16" s="66" t="s">
         <v>91</v>
@@ -3487,56 +3487,56 @@
       <c r="B23" s="10"/>
       <c r="AE23" s="6"/>
       <c r="AH23" s="64" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="10"/>
       <c r="AE24" s="6"/>
       <c r="AG24" s="66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="10"/>
       <c r="AE25" s="6"/>
       <c r="AH25" s="64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="10"/>
       <c r="AE26" s="6"/>
       <c r="AG26" s="66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="10"/>
       <c r="AE27" s="6"/>
       <c r="AH27" s="64" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="10"/>
       <c r="AE28" s="6"/>
       <c r="AG28" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="10"/>
       <c r="AE29" s="6"/>
       <c r="AH29" s="64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="10"/>
       <c r="AE30" s="6"/>
       <c r="AG30" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
@@ -3558,21 +3558,21 @@
       <c r="B33" s="10"/>
       <c r="AE33" s="6"/>
       <c r="AH33" s="64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="10"/>
       <c r="AE34" s="6"/>
       <c r="AG34" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="10"/>
       <c r="AE35" s="6"/>
       <c r="AH35" s="64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="2:34" ht="100" customHeight="1" x14ac:dyDescent="0.2">
@@ -3646,17 +3646,25 @@
     <row r="46" spans="2:34" ht="100" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="G10:I12"/>
     <mergeCell ref="R14:W16"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="C10:C11"/>
     <mergeCell ref="O10:Q10"/>
     <mergeCell ref="S9:S10"/>
     <mergeCell ref="O6:O7"/>
@@ -3664,17 +3672,9 @@
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="J8:M9"/>
-    <mergeCell ref="G10:I12"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="15" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -3813,10 +3813,10 @@
       <c r="X3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="Y3" s="103" t="s">
+      <c r="Y3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" s="104"/>
+      <c r="Z3" s="99"/>
       <c r="AA3" s="14" t="s">
         <v>0</v>
       </c>
@@ -4304,8 +4304,8 @@
       <c r="X10" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="Y10" s="83"/>
-      <c r="Z10" s="100"/>
+      <c r="Y10" s="93"/>
+      <c r="Z10" s="104"/>
       <c r="AA10" s="3" t="s">
         <v>0</v>
       </c>
@@ -4367,9 +4367,9 @@
       <c r="W11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="X11" s="84"/>
-      <c r="Y11" s="80"/>
-      <c r="Z11" s="85"/>
+      <c r="X11" s="94"/>
+      <c r="Y11" s="90"/>
+      <c r="Z11" s="95"/>
       <c r="AA11" s="3" t="s">
         <v>0</v>
       </c>
@@ -4431,9 +4431,9 @@
       <c r="W12" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="X12" s="84"/>
-      <c r="Y12" s="80"/>
-      <c r="Z12" s="85"/>
+      <c r="X12" s="94"/>
+      <c r="Y12" s="90"/>
+      <c r="Z12" s="95"/>
       <c r="AA12" s="19" t="s">
         <v>0</v>
       </c>
@@ -4525,14 +4525,14 @@
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="88" t="s">
+      <c r="J14" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
@@ -4550,12 +4550,12 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
@@ -4573,12 +4573,12 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="79"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="25"/>
@@ -4902,10 +4902,10 @@
       <c r="F3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="103" t="s">
+      <c r="G3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="104"/>
+      <c r="H3" s="99"/>
       <c r="I3" s="14" t="s">
         <v>0</v>
       </c>
@@ -5343,8 +5343,8 @@
       <c r="G10" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="83"/>
-      <c r="I10" s="100"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="104"/>
       <c r="J10" s="3" t="s">
         <v>0</v>
       </c>
@@ -5396,9 +5396,9 @@
       <c r="F11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="84"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="85"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="95"/>
       <c r="J11" s="3" t="s">
         <v>0</v>
       </c>
@@ -5453,9 +5453,9 @@
       <c r="F12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="84"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="85"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="95"/>
       <c r="J12" s="26" t="s">
         <v>44</v>
       </c>
@@ -5570,14 +5570,14 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="88" t="s">
+      <c r="R14" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="S14" s="88"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="88"/>
-      <c r="V14" s="88"/>
-      <c r="W14" s="88"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="79"/>
+      <c r="U14" s="79"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="79"/>
       <c r="AE14" s="6"/>
     </row>
     <row r="15" spans="2:31" ht="100" customHeight="1" x14ac:dyDescent="0.2">
@@ -5597,12 +5597,12 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="88"/>
-      <c r="U15" s="88"/>
-      <c r="V15" s="88"/>
-      <c r="W15" s="88"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="79"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="79"/>
       <c r="AE15" s="6"/>
     </row>
     <row r="16" spans="2:31" ht="100" customHeight="1" x14ac:dyDescent="0.2">
@@ -5622,12 +5622,12 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="88"/>
-      <c r="U16" s="88"/>
-      <c r="V16" s="88"/>
-      <c r="W16" s="88"/>
+      <c r="R16" s="79"/>
+      <c r="S16" s="79"/>
+      <c r="T16" s="79"/>
+      <c r="U16" s="79"/>
+      <c r="V16" s="79"/>
+      <c r="W16" s="79"/>
       <c r="AE16" s="6"/>
     </row>
     <row r="17" spans="2:31" ht="100" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>